<commit_message>
[anyce] - Future API
</commit_message>
<xml_diff>
--- a/Tutorial #/07. Asynchronous Programming.xlsx
+++ b/Tutorial #/07. Asynchronous Programming.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450235A4-EC89-4C6C-8A19-9F20205F011B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B837959-0509-4288-85CB-1850DFB66E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asynchronous Programming" sheetId="1" r:id="rId1"/>
+    <sheet name="Future" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Asynchronous Programming</t>
     <phoneticPr fontId="3"/>
@@ -50,13 +51,76 @@
   </si>
   <si>
     <t xml:space="preserve">එකම වේලාවකදී වෙන වෙනම run වෙන එක </t>
+  </si>
+  <si>
+    <t>Future</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Function එකක String එකක් return කරනකොට </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒ function එකේ return type එකත් String වෙන්න ඕනේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">සාමාන්‍ය විදියට String type return එකක් කරන්න බෑ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒත් flutter වලදී Asynchronous (anyce) වර්ගයේ function එකකින් </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Asynchronous (anyce) වර්ගයේ function එකකින් String type retun එකක් කරනවානම් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අනිවාර්යෙන්ම function retune type එකට future class එක add කරන්න ඕනේ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Asynchronous (anyce) function එකක result print කරමු</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">හරි result එකක් එන්නේ නැ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">එකට හේතුවක් වෙන්නේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asynchronous (anyce) function එක සාමාන්‍ය විදියට print කලොත් </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Asynchronous (anyce) function එක run වෙලා </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">result එක return කරන්න ටික වෙලාවක් යනවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒ නිසා අපි කරන්නේ function එකෙන් return එකක් එනකන් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">අපේ program එක hold කරලා තියාගන්නවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">await use කරනවානම් function එක අනිවාර්යෙන් anyce වෙන්න ඕනේ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">function එකක් anyce නම් future class එකක් use කරන්න ඕනේ </t>
+  </si>
+  <si>
+    <t>RUN</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +153,24 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF7030A0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF7030A0"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,10 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +213,539 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>415642</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>304230</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>507249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>350520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53177A94-BEFC-EA22-0750-3A7FEA876B55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="415642" y="3527490"/>
+          <a:ext cx="6019967" cy="3749610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>27762</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>199819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA1923D-40C8-EB4D-6637-760619CE87D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6827520" y="4655820"/>
+          <a:ext cx="6504762" cy="1647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>297180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>81823</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C243D4-78AE-7454-DC68-FB059CF19F2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="563880" y="8938260"/>
+          <a:ext cx="6787423" cy="1805940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>145830</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02499E3F-4D87-AB14-FD60-6A62B470F2F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="632460" y="12260580"/>
+          <a:ext cx="5441730" cy="3474720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>151881</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>268428</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C48E65B-D2CF-3FF9-E2C0-A5DC488ED470}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6621780" y="13380720"/>
+          <a:ext cx="4152381" cy="1419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>227971</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>287490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{191DF2D0-CEFB-CBE0-1AB2-B9197D931191}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1127760" y="18844260"/>
+          <a:ext cx="5028571" cy="1323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>449579</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>124724</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35556693-B9A7-8A0F-8C64-14056E0334CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1684019" y="21701760"/>
+          <a:ext cx="3698505" cy="1211580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219187</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CA1EA5C-320D-CA11-B428-9BB5ADC3D72E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1668780" y="23728680"/>
+          <a:ext cx="3808207" cy="899160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>251460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>14616</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>64639</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89FDAD93-1A22-9BBA-7E52-D0F7F2518C7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1623060" y="25481280"/>
+          <a:ext cx="4990476" cy="1047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>101956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>525781</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>203322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88219E12-B4ED-EDD1-4D9C-BF54DF4A8B9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670561" y="27389176"/>
+          <a:ext cx="5783580" cy="2981726"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>394872</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>525781</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>350296</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8BE6099-6602-6318-7885-B25E354191FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670561" y="30562452"/>
+          <a:ext cx="5783580" cy="1601344"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>358140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>159310</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>331268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5046B3B-E4CD-102A-9687-C7457FF4C260}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7117080" y="30525720"/>
+          <a:ext cx="5676190" cy="1619048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -452,4 +1069,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501EE77B-8AF6-4794-B005-07294640B859}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="2" max="2" width="7.3984375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="64.8" x14ac:dyDescent="1.55">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.8"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="B39" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="D43" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.8">
+      <c r="D44" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="B50" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="C51" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="B56" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="B60" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.8">
+      <c r="B65" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>